<commit_message>
gn: update result form
</commit_message>
<xml_diff>
--- a/LF/Confirmation/Ghana/gn_lf_pretas_3_resultat_fts_202210.xlsx
+++ b/LF/Confirmation/Ghana/gn_lf_pretas_3_resultat_fts_202210.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -331,13 +331,13 @@
     <t>Broken/partial control line</t>
   </si>
   <si>
-    <t>Difficulte.d’absorption.d’echantillon</t>
+    <t>Difficulte.d.absorption.d.echantillon</t>
   </si>
   <si>
     <t>Difficulty of absorbing sample</t>
   </si>
   <si>
-    <t>Difficulte.de.migration.d’echantillon</t>
+    <t>Difficulte.de.migration.d.echantillon</t>
   </si>
   <si>
     <t>Difficulty of migrating sample</t>
@@ -1420,7 +1420,7 @@
   <sheetPr/>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2007,10 +2007,10 @@
   <sheetPr/>
   <dimension ref="A1:F323"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>

</xml_diff>